<commit_message>
added searchterm.length<3 handling on API side as well (for postman testing) & testcases file completed
</commit_message>
<xml_diff>
--- a/testcasesForInstantSearch.xlsx
+++ b/testcasesForInstantSearch.xlsx
@@ -20,6 +20,7 @@
 <office:document-content xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:xforms="http://www.w3.org/2002/xforms" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:formx="urn:openoffice:names:experimental:ooxml-odf-interop:xmlns:form:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" office:version="1.2">
   <office:scripts/>
   <office:font-face-decls>
+    <style:font-face style:name="Ubuntu" svg:font-family="Ubuntu" style:font-pitch="variable"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="FreeSans" svg:font-family="FreeSans" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -27,13 +28,13 @@
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="24.5mm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="12.79mm"/>
     </style:style>
     <style:style style:name="co2" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="62.09mm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="297.11mm"/>
     </style:style>
     <style:style style:name="co3" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="73.8mm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="211.05mm"/>
     </style:style>
     <style:style style:name="co4" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="54.45mm"/>
@@ -42,10 +43,43 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="22.58mm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
+      <style:table-row-properties style:row-height="10.57mm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+    </style:style>
+    <style:style style:name="ro2" style:family="table-row">
+      <style:table-row-properties style:row-height="5.54mm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+    </style:style>
+    <style:style style:name="ro3" style:family="table-row">
+      <style:table-row-properties style:row-height="4.48mm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+    </style:style>
+    <style:style style:name="ro4" style:family="table-row">
+      <style:table-row-properties style:row-height="5.01mm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+    </style:style>
+    <style:style style:name="ro5" style:family="table-row">
+      <style:table-row-properties style:row-height="4.74mm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+    </style:style>
+    <style:style style:name="ro6" style:family="table-row">
       <style:table-row-properties style:row-height="4.52mm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
+    </style:style>
+    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties style:font-name="Liberation Sans" style:font-name-asian="Noto Sans CJK SC Regular" style:font-name-complex="FreeSans"/>
+    </style:style>
+    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties style:use-window-font-color="true" style:font-name="Liberation Sans" fo:font-size="10pt" fo:language="en" fo:country="IN" style:font-name-asian="Noto Sans CJK SC Regular" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-name-complex="FreeSans" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN"/>
+    </style:style>
+    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties style:use-window-font-color="true" style:font-name="Liberation Sans" fo:language="en" fo:country="IN" style:font-name-asian="Noto Sans CJK SC Regular" style:language-asian="zh" style:country-asian="CN" style:font-name-complex="FreeSans" style:language-complex="hi" style:country-complex="IN"/>
+    </style:style>
+    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" style:font-name="Liberation Sans" fo:language="none" fo:country="none" style:font-name-asian="Ubuntu" style:language-asian="none" style:country-asian="none" style:font-name-complex="Ubuntu" style:language-complex="none" style:country-complex="none"/>
+    </style:style>
+    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#3c3c3c" style:font-name="Liberation Sans" fo:language="none" fo:country="none" style:font-name-asian="Ubuntu" style:language-asian="none" style:country-asian="none" style:font-name-complex="Ubuntu" style:language-complex="none" style:country-complex="none"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
@@ -57,18 +91,241 @@
         <table:table-column table:style-name="co3" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Sr. No.</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Scenario</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>Expected Result</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Example</text:p>
-          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>User Types a String with characters&gt;=3 &amp; taps/clicks on search</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Search Results must be displayed</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>User Types a String with characters&lt;3 &amp; taps/clicks on search</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Alert displaying the message “Search Term must be &gt;= 3 characters” pops up</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="float" office:value="3" calcext:value-type="float">
+            <text:p>3</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Resultant String Starts with the search term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Resultant string gets HIGHER priority &amp; appears TOWARDS the TOP</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="float" office:value="4" calcext:value-type="float">
+            <text:p>4</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Resultant String does not start with the search term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Resultant string gets LOWER priority &amp; appears AFTER the resultant strings starting with the search term</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="float" office:value="5" calcext:value-type="float">
+            <text:p>5</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is shorter in length than the Next Resultant String</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current resultant string will be given MORE priority &amp; will be shown ABOVE the next resultant string in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro4">
+          <table:table-cell office:value-type="float" office:value="6" calcext:value-type="float">
+            <text:p>6</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is longer in length than the Next Resultant String</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Current resultant string will be given LESSER priority &amp; will be shown BELOW the next resultant string in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro5">
+          <table:table-cell office:value-type="float" office:value="7" calcext:value-type="float">
+            <text:p>7</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is shorter in length than the Next Resultant String &amp; both strings start with the Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given MORE priority &amp; will be shown ABOVE the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="8" calcext:value-type="float">
+            <text:p>8</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is shorter in length than the Next Resultant String &amp; Current Resultant string starts with the Search Term, but Next Resultant String does not start with Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given MORE priority &amp; will be shown ABOVE the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="9" calcext:value-type="float">
+            <text:p>9</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is shorter in length than the Next Resultant String &amp; both strings DO NOT start with the Search Term </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given MORE priority &amp; will be shown ABOVE the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="10" calcext:value-type="float">
+            <text:p>10</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is longer in length than the Next Resultant String &amp; Current Resultant string starts with the Search Term, but Next Resultant String does not start with Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given MORE priority &amp; will be shown ABOVE the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="11" calcext:value-type="float">
+            <text:p>11</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String &amp; Next Resultant String are equal in length &amp; Current Resultant string starts with the Search Term, but Next Resultant String does not start with Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given MORE priority &amp; will be shown ABOVE the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="12" calcext:value-type="float">
+            <text:p>12</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is shorter in length than the Next Resultant String &amp; Current Resultant string does not start with the Search Term, but Next Resultant String starts with Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given LESSER priority &amp; will be shown BELOW the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="13" calcext:value-type="float">
+            <text:p>13</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is longer in length than the Next Resultant String &amp; both strings start with the Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given LESSER priority &amp; will be shown BELOW the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="14" calcext:value-type="float">
+            <text:p>14</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is longer in length than the Next Resultant String &amp; Current Resultant string does not start with the Search Term, but Next Resultant String starts with Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given LESSER priority &amp; will be shown BELOW the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="15" calcext:value-type="float">
+            <text:p>15</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String is longer in length than the Next Resultant String &amp; both strings DO NOT start with the Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given LESSER priority &amp; will be shown BELOW the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="16" calcext:value-type="float">
+            <text:p>16</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String &amp; Next Resultant String are equal in length &amp; Current Resultant string does not start with the Search Term, but Next Resultant String starts with Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String will be given LESSER priority &amp; will be shown BELOW the Next Resultant String in the list</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="17" calcext:value-type="float">
+            <text:p>17</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String &amp; Next Resultant String are equal in length &amp; both strings start with the Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+            <text:p>Both Current Resultant String &amp; Next Resultant String will be given same priority</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell office:value-type="float" office:value="18" calcext:value-type="float">
+            <text:p>18</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Current Resultant String &amp; Next Resultant String are equal in length &amp; both strings DO NOT start with the Search Term</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Both Current Resultant String &amp; Next Resultant String will be given same priority</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6" table:number-rows-repeated="5">
+          <table:table-cell table:number-columns-repeated="4"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro6">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce6"/>
+          <table:table-cell table:style-name="ce2"/>
+          <table:table-cell/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -82,10 +339,10 @@
   <office:meta>
     <meta:creation-date>2019-02-09T02:05:55.014906914</meta:creation-date>
     <meta:generator>LibreOffice/5.1.6.2$Linux_X86_64 LibreOffice_project/10m0$Build-2</meta:generator>
-    <dc:date>2019-02-09T02:13:31.199965943</dc:date>
-    <meta:editing-duration>PT7M37S</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="4" meta:object-count="0"/>
+    <dc:date>2019-02-09T14:32:19.053091060</dc:date>
+    <meta:editing-duration>PT13M8S</meta:editing-duration>
+    <meta:editing-cycles>2</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="57" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -96,15 +353,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">21484</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">451</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">52094</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">9450</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">6</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -146,6 +403,7 @@
       </config:config-item-map-indexed>
     </config:config-item-set>
     <config:config-item-set config:name="ooo:configuration-settings">
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="IsDocumentShared" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="AllowPrintJobCancel" config:type="boolean">true</config:config-item>
@@ -165,13 +423,22 @@
       <config:config-item config:name="SaveVersionOnClose" config:type="boolean">false</config:config-item>
       <config:config-item config:name="GridColor" config:type="long">12632256</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
+      <config:config-item-map-indexed config:name="ForbiddenCharacters">
+        <config:config-item-map-entry>
+          <config:config-item config:name="Language" config:type="string">en</config:config-item>
+          <config:config-item config:name="Country" config:type="string">IN</config:config-item>
+          <config:config-item config:name="Variant" config:type="string"/>
+          <config:config-item config:name="BeginLine" config:type="string"/>
+          <config:config-item config:name="EndLine" config:type="string"/>
+        </config:config-item-map-entry>
+      </config:config-item-map-indexed>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="RasterSubdivisionX" config:type="int">1</config:config-item>
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="RasterSubdivisionY" config:type="int">1</config:config-item>
       <config:config-item config:name="AutoCalculate" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">gAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMApgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCm1hcmdpbmRhanVzdG1lbnQ9MCwwLDAsMApjb2xvcmRlcHRoPTI0CnBzbGV2ZWw9MApwZGZkZXZpY2U9MApjb2xvcmRldmljZT0wClBQRENvbnRleERhdGEKUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFCgBEVVBMRVhfT0ZG</config:config-item>
       <config:config-item config:name="ApplyUserData" config:type="boolean">true</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
     </config:config-item-set>
@@ -182,6 +449,7 @@
 <file path=styles.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-styles xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:style="urn:oasis:names:tc:opendocument:xmlns:style:1.0" xmlns:text="urn:oasis:names:tc:opendocument:xmlns:text:1.0" xmlns:table="urn:oasis:names:tc:opendocument:xmlns:table:1.0" xmlns:draw="urn:oasis:names:tc:opendocument:xmlns:drawing:1.0" xmlns:fo="urn:oasis:names:tc:opendocument:xmlns:xsl-fo-compatible:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:number="urn:oasis:names:tc:opendocument:xmlns:datastyle:1.0" xmlns:presentation="urn:oasis:names:tc:opendocument:xmlns:presentation:1.0" xmlns:svg="urn:oasis:names:tc:opendocument:xmlns:svg-compatible:1.0" xmlns:chart="urn:oasis:names:tc:opendocument:xmlns:chart:1.0" xmlns:dr3d="urn:oasis:names:tc:opendocument:xmlns:dr3d:1.0" xmlns:math="http://www.w3.org/1998/Math/MathML" xmlns:form="urn:oasis:names:tc:opendocument:xmlns:form:1.0" xmlns:script="urn:oasis:names:tc:opendocument:xmlns:script:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:ooow="http://openoffice.org/2004/writer" xmlns:oooc="http://openoffice.org/2004/calc" xmlns:dom="http://www.w3.org/2001/xml-events" xmlns:rpt="http://openoffice.org/2005/report" xmlns:of="urn:oasis:names:tc:opendocument:xmlns:of:1.2" xmlns:xhtml="http://www.w3.org/1999/xhtml" xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:tableooo="http://openoffice.org/2009/table" xmlns:drawooo="http://openoffice.org/2010/draw" xmlns:calcext="urn:org:documentfoundation:names:experimental:calc:xmlns:calcext:1.0" xmlns:loext="urn:org:documentfoundation:names:experimental:office:xmlns:loext:1.0" xmlns:field="urn:openoffice:names:experimental:ooo-ms-interop:xmlns:field:1.0" xmlns:css3t="http://www.w3.org/TR/css3-text/" office:version="1.2">
   <office:font-face-decls>
+    <style:font-face style:name="Ubuntu" svg:font-family="Ubuntu" style:font-pitch="variable"/>
     <style:font-face style:name="Liberation Sans" svg:font-family="'Liberation Sans'" style:font-family-generic="swiss" style:font-pitch="variable"/>
     <style:font-face style:name="DejaVu Sans" svg:font-family="'DejaVu Sans'" style:font-family-generic="system" style:font-pitch="variable"/>
     <style:font-face style:name="FreeSans" svg:font-family="FreeSans" style:font-family-generic="system" style:font-pitch="variable"/>
@@ -276,7 +544,7 @@
           <text:p>
             <text:date style:data-style-name="N2" text:date-value="2019-02-09">00/00/0000</text:date>
             , 
-            <text:time>00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="13:24:35.594478619">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>